<commit_message>
created regular proposal page obj and log4j updates
</commit_message>
<xml_diff>
--- a/caphase3/src/test/java/com/softweb/cure/excels/ProjectFundingData.xlsx
+++ b/caphase3/src/test/java/com/softweb/cure/excels/ProjectFundingData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13950" windowHeight="6780"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="18030" windowHeight="10260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:R32"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>ExistingProjFund</t>
   </si>
@@ -53,19 +53,31 @@
   </si>
   <si>
     <t>126756</t>
+  </si>
+  <si>
+    <t>SpeedUp</t>
+  </si>
+  <si>
+    <t>"Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,9 +100,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +423,7 @@
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -470,13 +483,85 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>